<commit_message>
Updated Pick-up Items work sheet.
</commit_message>
<xml_diff>
--- a/Project Documents/Pick-up Items.xlsx
+++ b/Project Documents/Pick-up Items.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00195238\Documents\Push-Penguin-3D\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
-  <si>
-    <t>Emmet Bolger -T00195238</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Job: Pick-up Items</t>
   </si>
@@ -35,24 +32,15 @@
     <t xml:space="preserve">Item Name </t>
   </si>
   <si>
-    <t>Eg. Penguin/Player</t>
-  </si>
-  <si>
     <t>Describe Role in game</t>
   </si>
   <si>
-    <t>Text description of role in game</t>
-  </si>
-  <si>
     <t>Internal Functionality</t>
   </si>
   <si>
     <t>Text Description</t>
   </si>
   <si>
-    <t>Eg Turn Left</t>
-  </si>
-  <si>
     <t>External Outgoing</t>
   </si>
   <si>
@@ -62,22 +50,37 @@
     <t>Communication with?</t>
   </si>
   <si>
-    <t>Eg Push</t>
-  </si>
-  <si>
     <t>External Incoming</t>
   </si>
   <si>
     <t xml:space="preserve">Return </t>
   </si>
   <si>
-    <t>ShouldTurnLeft</t>
-  </si>
-  <si>
     <t xml:space="preserve">Name of InterFace </t>
   </si>
   <si>
     <t>https://unity3d.com/learn/tutorials/topics/scripting/interfaces</t>
+  </si>
+  <si>
+    <t>Laura Braak - T00198405</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Charakter picks up the Items to earn score. </t>
+  </si>
+  <si>
+    <t>Default Constructer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating Default Item with a default Value </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collecting Animation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When collusion with penguin, start a animation </t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,85 +425,86 @@
   <sheetData>
     <row r="1" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
         <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
         <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Pick-up Items exel-sheet.
</commit_message>
<xml_diff>
--- a/Project Documents/Pick-up Items.xlsx
+++ b/Project Documents/Pick-up Items.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00198405\Desktop\GD\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Job: Pick-up Items</t>
   </si>
@@ -53,9 +53,6 @@
     <t>External Incoming</t>
   </si>
   <si>
-    <t xml:space="preserve">Return </t>
-  </si>
-  <si>
     <t xml:space="preserve">Name of InterFace </t>
   </si>
   <si>
@@ -71,16 +68,64 @@
     <t xml:space="preserve">The Charakter picks up the Items to earn score. </t>
   </si>
   <si>
-    <t>Default Constructer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creating Default Item with a default Value </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collecting Animation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When collusion with penguin, start a animation </t>
+    <t>Return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value </t>
+  </si>
+  <si>
+    <t>getValue()</t>
+  </si>
+  <si>
+    <t>setValue()</t>
+  </si>
+  <si>
+    <t>returns the current value of the Item.</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>true/false</t>
+  </si>
+  <si>
+    <t>startCollusionAnimation();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When collusion with something animate. If collusion is with Penguin get bigger and disappear. Else rotate. </t>
+  </si>
+  <si>
+    <t>Destruct</t>
+  </si>
+  <si>
+    <t>object destroys itself</t>
+  </si>
+  <si>
+    <t>Gamemanager</t>
+  </si>
+  <si>
+    <t>reportCollection()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value, Position </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value Position </t>
+  </si>
+  <si>
+    <t>reports the collection to the Popup-Score and gives him current Position and Value.</t>
+  </si>
+  <si>
+    <t>Popup-Score</t>
+  </si>
+  <si>
+    <t>Constructer</t>
+  </si>
+  <si>
+    <t>Gamemanager sets the value to the item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating Constructor </t>
   </si>
 </sst>
 </file>
@@ -409,45 +454,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.28515625" customWidth="1"/>
-    <col min="2" max="2" width="63" customWidth="1"/>
+    <col min="2" max="2" width="95.42578125" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -455,15 +500,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -474,18 +535,44 @@
         <v>6</v>
       </c>
       <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -493,18 +580,38 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>